<commit_message>
Notebook and files update
Results now include distribution embodied
</commit_message>
<xml_diff>
--- a/data/processed/lca/appliance embedded emissions incl. multisplits.xlsx
+++ b/data/processed/lca/appliance embedded emissions incl. multisplits.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\engfs\enel\EPECentre\EPECentre\Research\Other Projects\2024 - EECA Residential Space &amp; Water Heating\products\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\engfs\enel\epecentre\epecentre\Research\Other Projects\2024 - EECA Residential Space &amp; Water Heating\products\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CF54F3-BC81-45F0-A215-A5D1E7E72586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4773D83-3E98-4DDA-AE71-07869EE0F23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{27AF100B-5109-46AD-9AE0-EF3B7EF58B86}"/>
   </bookViews>
@@ -18,8 +18,14 @@
     <sheet name="Installation" sheetId="4" r:id="rId3"/>
     <sheet name="EOL" sheetId="6" r:id="rId4"/>
     <sheet name="B2-B5" sheetId="7" r:id="rId5"/>
-    <sheet name="Key" sheetId="2" r:id="rId6"/>
+    <sheet name="weight" sheetId="8" r:id="rId6"/>
+    <sheet name="Key" sheetId="2" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="SHIP_DWR_SHDWBUF_em_t">Key!$H$27</definedName>
+    <definedName name="SHIP_OTHER_em_t">Key!$I$27</definedName>
+    <definedName name="TRUCK_em_t">Key!$I$28</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="38">
   <si>
     <t>SH-R</t>
   </si>
@@ -129,6 +135,33 @@
   <si>
     <t>Mass-H1-CH-HPb</t>
   </si>
+  <si>
+    <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>Shipping Distances (km)</t>
+  </si>
+  <si>
+    <t>DW-R/SHDW-BUF</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>Trucking Distances (km)</t>
+  </si>
+  <si>
+    <t>Emissions kgCO2e/tkm Ship</t>
+  </si>
+  <si>
+    <t>Emissions kgCO2e/tkm Truck</t>
+  </si>
+  <si>
+    <t>Emissions kGCO2e/t (ship)</t>
+  </si>
+  <si>
+    <t>Emissions kGCO2e/t (truck)</t>
+  </si>
 </sst>
 </file>
 
@@ -174,10 +207,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -186,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -196,6 +238,12 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F43AA1-1492-4CC0-963B-2BA3D20F19E1}">
   <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -760,7 +808,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4">
-        <v>608</v>
+        <v>771</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1141,10 +1189,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="3">
-        <v>530</v>
+        <v>678</v>
       </c>
       <c r="D24" s="3">
-        <v>1216</v>
+        <v>1565</v>
       </c>
     </row>
   </sheetData>
@@ -1160,7 +1208,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1214,32 +1262,41 @@
       <c r="B3">
         <v>17</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
+      <c r="C3" s="9">
+        <f>weight!C3*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>3.0245574743999999</v>
+      </c>
+      <c r="D3" s="9">
+        <f>weight!D3*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>3.8928783940200007</v>
+      </c>
+      <c r="E3" s="9">
+        <f>weight!E3*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>4.7611993136400006</v>
+      </c>
+      <c r="F3" s="9">
+        <f>weight!F3*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>5.6295202332600001</v>
+      </c>
+      <c r="G3" s="9">
+        <f>weight!G3*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>6.4978411528800004</v>
+      </c>
+      <c r="H3" s="9">
+        <f>weight!H3*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>7.3661620724999999</v>
+      </c>
+      <c r="I3" s="9">
+        <f>weight!I3*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>8.2344829921200002</v>
+      </c>
+      <c r="J3" s="9">
+        <f>weight!J3*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>9.1028039117400006</v>
+      </c>
+      <c r="K3" s="9">
+        <f>weight!K3*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>9.9711248313600009</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -1305,35 +1362,54 @@
       <c r="B6">
         <v>17</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
+        <f>weight!H6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>9.1947968640250384</v>
+      </c>
+      <c r="I6" s="9">
+        <f>weight!I6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>9.8824847924880004</v>
+      </c>
+      <c r="J6" s="9">
+        <f>weight!J6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>11.080266056244</v>
+      </c>
+      <c r="K6" s="9">
+        <f>weight!K6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.278047319999999</v>
+      </c>
+      <c r="L6" s="9">
+        <f>weight!L6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.278047319999999</v>
+      </c>
+      <c r="M6" s="9">
+        <f>weight!M6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.278047319999999</v>
+      </c>
+      <c r="N6" s="9">
+        <f>weight!N6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.278047319999999</v>
+      </c>
+      <c r="O6" s="9">
+        <f>weight!O6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.278047319999999</v>
+      </c>
+      <c r="P6" s="9">
+        <f>weight!P6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.278047319999999</v>
+      </c>
+      <c r="Q6" s="9">
+        <f>weight!Q6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.278047319999999</v>
+      </c>
+      <c r="R6" s="9">
+        <f>weight!R6*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.278047319999999</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
@@ -1346,21 +1422,633 @@
       <c r="B7">
         <v>17</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
+        <f>weight!C7*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>6.2189819999999996</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
+        <f>weight!E7*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>6.2189819999999996</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9">
+        <f>weight!G7*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>9.2396303999999994</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9">
+        <f>weight!M7*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>15.991668000000001</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>17</v>
+      </c>
+      <c r="C8" s="9">
+        <f>weight!C8*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.437963999999999</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
+        <f>weight!E8*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.437963999999999</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
+        <f>weight!I8*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>12.437963999999999</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9">
+        <f>weight!L8*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>20.433798000000003</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>135</v>
+      </c>
+      <c r="D11">
+        <f>C11*1.2</f>
+        <v>162</v>
+      </c>
+      <c r="E11">
+        <v>180</v>
+      </c>
+      <c r="F11">
+        <f>E11*1.2</f>
+        <v>216</v>
+      </c>
+      <c r="G11">
+        <v>300</v>
+      </c>
+      <c r="H11">
+        <f>G11*1.2</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12" s="9">
+        <f>weight!C12*(SHIP_DWR_SHDWBUF_em_t+TRUCK_em_t)/1000</f>
+        <v>3.1272393599999999</v>
+      </c>
+      <c r="D12" s="9">
+        <f>weight!D12*(SHIP_DWR_SHDWBUF_em_t+TRUCK_em_t)/1000</f>
+        <v>3.5200637579520002</v>
+      </c>
+      <c r="E12" s="9">
+        <f>weight!E12*(SHIP_DWR_SHDWBUF_em_t+TRUCK_em_t)/1000</f>
+        <v>3.8820902400000001</v>
+      </c>
+      <c r="F12" s="9">
+        <f>weight!F12*(SHIP_DWR_SHDWBUF_em_t+TRUCK_em_t)/1000</f>
+        <v>4.4212694399999997</v>
+      </c>
+      <c r="G12" s="9">
+        <f>weight!G12*(SHIP_DWR_SHDWBUF_em_t+TRUCK_em_t)/1000</f>
+        <v>5.6074636799999995</v>
+      </c>
+      <c r="H12" s="9">
+        <f>weight!H12*(SHIP_DWR_SHDWBUF_em_t+TRUCK_em_t)/1000</f>
+        <v>6.5779862400000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>135</v>
+      </c>
+      <c r="D14">
+        <f>C14*1.2</f>
+        <v>162</v>
+      </c>
+      <c r="E14">
+        <v>180</v>
+      </c>
+      <c r="F14">
+        <f>E14*1.2</f>
+        <v>216</v>
+      </c>
+      <c r="G14">
+        <v>300</v>
+      </c>
+      <c r="H14">
+        <f>G14*1.2</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15" s="9">
+        <f>weight!C15*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>11.30195144232</v>
+      </c>
+      <c r="D15" s="9">
+        <f>weight!D15*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>13.693505391720002</v>
+      </c>
+      <c r="E15" s="9">
+        <f>weight!E15*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>15.287874691320001</v>
+      </c>
+      <c r="F15" s="9">
+        <f>weight!F15*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>18.476613290520003</v>
+      </c>
+      <c r="G15" s="9">
+        <f>weight!G15*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>25.917003355320006</v>
+      </c>
+      <c r="H15" s="9">
+        <f>weight!H15*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>31.231567687320002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <f>D17+1</f>
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:N17" si="1">E17+1</f>
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="9">
+        <f>weight!C18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>44.174761785000001</v>
+      </c>
+      <c r="D18" s="9">
+        <f>weight!D18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>45.067541072400005</v>
+      </c>
+      <c r="E18" s="9">
+        <f>weight!E18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>45.960320359800001</v>
+      </c>
+      <c r="F18" s="9">
+        <f>weight!F18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>46.853099647200011</v>
+      </c>
+      <c r="G18" s="9">
+        <f>weight!G18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>47.745878934600007</v>
+      </c>
+      <c r="H18" s="9">
+        <f>weight!H18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>48.638658222000004</v>
+      </c>
+      <c r="I18" s="9">
+        <f>weight!I18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>49.531437509400007</v>
+      </c>
+      <c r="J18" s="9">
+        <f>weight!J18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>50.424216796799996</v>
+      </c>
+      <c r="K18" s="9">
+        <f>weight!K18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>51.316996084199999</v>
+      </c>
+      <c r="L18" s="9">
+        <f>weight!L18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>52.209775371600003</v>
+      </c>
+      <c r="M18" s="9">
+        <f>weight!M18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>53.102554659000006</v>
+      </c>
+      <c r="N18" s="9">
+        <f>weight!N18*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>53.995333946400002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>C20+1</f>
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20:G20" si="2">D20+1</f>
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21" s="9">
+        <f>weight!C21*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>3.2338706400000001</v>
+      </c>
+      <c r="D21" s="9">
+        <f>weight!D21*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>3.2338706400000001</v>
+      </c>
+      <c r="E21" s="9">
+        <f>weight!E21*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>3.5892410400000001</v>
+      </c>
+      <c r="F21" s="9">
+        <f>weight!F21*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>3.8557688400000001</v>
+      </c>
+      <c r="G21" s="9">
+        <f>weight!G21*(SHIP_OTHER_em_t+TRUCK_em_t)/1000</f>
+        <v>4.83303744</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>300</v>
+      </c>
+      <c r="D23">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24" s="9">
+        <f>weight!C24*(SHIP_DWR_SHDWBUF_em_t+TRUCK_em_t)/1000</f>
+        <v>7.8180984000000011</v>
+      </c>
+      <c r="D24" s="9">
+        <f>weight!D24*(SHIP_DWR_SHDWBUF_em_t+TRUCK_em_t)/1000</f>
+        <v>15.636196800000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414EA997-C34B-492F-B371-77D1D2B6D5A3}">
+  <dimension ref="A1:U24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1.5</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2.5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>3.5</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>4.5</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2">
-        <v>0</v>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.17386757142857118</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.22378325357142828</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.27369893571428533</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.32361461785714241</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.37353029999999948</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0.4234459821428565</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.47336166428571363</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.52327734642857071</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0.57319302857142773</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <f>I5+0.5</f>
+        <v>5.5</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:R5" si="0">J5+0.5</f>
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="H6" s="3">
+        <v>19</v>
+      </c>
+      <c r="I6" s="7">
+        <v>21</v>
+      </c>
+      <c r="J6" s="7">
+        <v>23</v>
+      </c>
+      <c r="K6" s="7">
+        <v>26</v>
+      </c>
+      <c r="L6" s="7">
+        <v>26</v>
+      </c>
+      <c r="M6" s="7">
+        <v>26</v>
+      </c>
+      <c r="N6" s="7">
+        <v>26</v>
+      </c>
+      <c r="O6" s="7">
+        <v>26</v>
+      </c>
+      <c r="P6" s="7">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>26</v>
+      </c>
+      <c r="R6" s="7">
+        <v>26</v>
+      </c>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3">
+        <v>25.7</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
+        <v>25.7</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4">
+        <v>33</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1378,21 +2066,25 @@
       <c r="B8">
         <v>17</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2"/>
+      <c r="C8" s="3">
+        <v>51.3</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>51.3</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4">
+        <v>51.3</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4">
+        <v>37.6</v>
+      </c>
+      <c r="M8" s="4"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
@@ -1460,23 +2152,23 @@
       <c r="B12">
         <v>17</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
+      <c r="C12" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -1515,23 +2207,23 @@
       <c r="B15">
         <v>17</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
+      <c r="C15" s="5">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D15" s="5">
+        <v>11.8</v>
+      </c>
+      <c r="E15" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="F15" s="5">
+        <v>16.8</v>
+      </c>
+      <c r="G15" s="5">
+        <v>24.5</v>
+      </c>
+      <c r="H15" s="5">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
@@ -1595,41 +2287,41 @@
       <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
+      <c r="C18" s="7">
+        <v>31.036000000000005</v>
+      </c>
+      <c r="D18" s="7">
+        <v>41.665999999999997</v>
+      </c>
+      <c r="E18" s="7">
+        <v>52.296000000000006</v>
+      </c>
+      <c r="F18" s="7">
+        <v>62.926000000000002</v>
+      </c>
+      <c r="G18" s="7">
+        <v>73.555999999999997</v>
+      </c>
+      <c r="H18" s="7">
+        <v>84.186000000000007</v>
+      </c>
+      <c r="I18" s="7">
+        <v>94.816000000000003</v>
+      </c>
+      <c r="J18" s="7">
+        <v>105.446</v>
+      </c>
+      <c r="K18" s="7">
+        <v>116.07599999999999</v>
+      </c>
+      <c r="L18" s="7">
+        <v>126.70600000000002</v>
+      </c>
+      <c r="M18" s="7">
+        <v>137.33600000000001</v>
+      </c>
+      <c r="N18" s="7">
+        <v>147.96600000000001</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -1666,23 +2358,20 @@
       <c r="B21">
         <v>16</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
+      <c r="C21" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="F21" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G21" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -1706,11 +2395,11 @@
       <c r="B24">
         <v>22</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
+      <c r="C24" s="3">
+        <v>12</v>
+      </c>
+      <c r="D24" s="3">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1718,15 +2407,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414EA997-C34B-492F-B371-77D1D2B6D5A3}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F74B9C2-1E78-4E89-B2C0-D50E247C4205}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1778,31 +2470,31 @@
         <v>17</v>
       </c>
       <c r="C3" s="8">
-        <v>0.17386757142857118</v>
+        <v>4.8634285714285754</v>
       </c>
       <c r="D3" s="8">
-        <v>0.22378325357142828</v>
+        <v>6.2596714285714343</v>
       </c>
       <c r="E3" s="8">
-        <v>0.27369893571428533</v>
+        <v>7.6559142857142923</v>
       </c>
       <c r="F3" s="8">
-        <v>0.32361461785714241</v>
+        <v>9.0521571428571512</v>
       </c>
       <c r="G3" s="8">
-        <v>0.37353029999999948</v>
+        <v>10.44840000000001</v>
       </c>
       <c r="H3" s="8">
-        <v>0.4234459821428565</v>
+        <v>11.844642857142867</v>
       </c>
       <c r="I3" s="8">
-        <v>0.47336166428571363</v>
+        <v>13.240885714285726</v>
       </c>
       <c r="J3" s="8">
-        <v>0.52327734642857071</v>
+        <v>14.637128571428585</v>
       </c>
       <c r="K3" s="8">
-        <v>0.57319302857142773</v>
+        <v>16.033371428571442</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -1869,37 +2561,37 @@
         <v>17</v>
       </c>
       <c r="H6" s="3">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="I6" s="7">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="J6" s="7">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="K6" s="7">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="L6" s="7">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="M6" s="7">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="N6" s="7">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="O6" s="7">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="P6" s="7">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="Q6" s="7">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="R6" s="7">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
@@ -1913,15 +2605,15 @@
         <v>17</v>
       </c>
       <c r="C7" s="3">
-        <v>25.7</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3">
-        <v>25.7</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3">
-        <v>19.100000000000001</v>
+        <v>90.1</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="4"/>
@@ -1929,7 +2621,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4">
-        <v>26.9</v>
+        <v>266</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1948,22 +2640,22 @@
         <v>17</v>
       </c>
       <c r="C8" s="3">
-        <v>51.3</v>
+        <v>152.1</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3">
-        <v>51.3</v>
+        <v>152.1</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="4">
-        <v>51.3</v>
+      <c r="I8" s="3">
+        <v>152.1</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4">
-        <v>37.6</v>
+        <v>219.7</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="2"/>
@@ -2034,579 +2726,6 @@
         <v>17</v>
       </c>
       <c r="C12" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="D12" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="E12" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="F12" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="G12" s="3">
-        <v>5</v>
-      </c>
-      <c r="H12" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>135</v>
-      </c>
-      <c r="D14">
-        <f>C14*1.2</f>
-        <v>162</v>
-      </c>
-      <c r="E14">
-        <v>180</v>
-      </c>
-      <c r="F14">
-        <f>E14*1.2</f>
-        <v>216</v>
-      </c>
-      <c r="G14">
-        <v>300</v>
-      </c>
-      <c r="H14">
-        <f>G14*1.2</f>
-        <v>360</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15">
-        <v>17</v>
-      </c>
-      <c r="C15" s="5">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="D15" s="5">
-        <v>11.8</v>
-      </c>
-      <c r="E15" s="5">
-        <v>13.5</v>
-      </c>
-      <c r="F15" s="5">
-        <v>16.8</v>
-      </c>
-      <c r="G15" s="5">
-        <v>24.5</v>
-      </c>
-      <c r="H15" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="D17">
-        <v>6</v>
-      </c>
-      <c r="E17">
-        <f>D17+1</f>
-        <v>7</v>
-      </c>
-      <c r="F17">
-        <f t="shared" ref="F17:N17" si="1">E17+1</f>
-        <v>8</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" s="7">
-        <v>31.036000000000005</v>
-      </c>
-      <c r="D18" s="7">
-        <v>41.665999999999997</v>
-      </c>
-      <c r="E18" s="7">
-        <v>52.296000000000006</v>
-      </c>
-      <c r="F18" s="7">
-        <v>62.926000000000002</v>
-      </c>
-      <c r="G18" s="7">
-        <v>73.555999999999997</v>
-      </c>
-      <c r="H18" s="7">
-        <v>84.186000000000007</v>
-      </c>
-      <c r="I18" s="7">
-        <v>94.816000000000003</v>
-      </c>
-      <c r="J18" s="7">
-        <v>105.446</v>
-      </c>
-      <c r="K18" s="7">
-        <v>116.07599999999999</v>
-      </c>
-      <c r="L18" s="7">
-        <v>126.70600000000002</v>
-      </c>
-      <c r="M18" s="7">
-        <v>137.33600000000001</v>
-      </c>
-      <c r="N18" s="7">
-        <v>147.96600000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <f>C20+1</f>
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <f t="shared" ref="E20:G20" si="2">D20+1</f>
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21">
-        <v>16</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="D21" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="E21" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="F21" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="G21" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23">
-        <v>300</v>
-      </c>
-      <c r="D23">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24">
-        <v>22</v>
-      </c>
-      <c r="C24" s="3">
-        <v>12</v>
-      </c>
-      <c r="D24" s="3">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F74B9C2-1E78-4E89-B2C0-D50E247C4205}">
-  <dimension ref="A1:U24"/>
-  <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1.5</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>2.5</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>3.5</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>4.5</v>
-      </c>
-      <c r="K2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>17</v>
-      </c>
-      <c r="C3" s="8">
-        <v>4.8634285714285754</v>
-      </c>
-      <c r="D3" s="8">
-        <v>6.2596714285714343</v>
-      </c>
-      <c r="E3" s="8">
-        <v>7.6559142857142923</v>
-      </c>
-      <c r="F3" s="8">
-        <v>9.0521571428571512</v>
-      </c>
-      <c r="G3" s="8">
-        <v>10.44840000000001</v>
-      </c>
-      <c r="H3" s="8">
-        <v>11.844642857142867</v>
-      </c>
-      <c r="I3" s="8">
-        <v>13.240885714285726</v>
-      </c>
-      <c r="J3" s="8">
-        <v>14.637128571428585</v>
-      </c>
-      <c r="K3" s="8">
-        <v>16.033371428571442</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <f>I5+0.5</f>
-        <v>5.5</v>
-      </c>
-      <c r="K5">
-        <f t="shared" ref="K5:R5" si="0">J5+0.5</f>
-        <v>6</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="R5">
-        <f t="shared" si="0"/>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>17</v>
-      </c>
-      <c r="H6" s="3">
-        <v>86</v>
-      </c>
-      <c r="I6" s="7">
-        <v>92</v>
-      </c>
-      <c r="J6" s="7">
-        <v>104</v>
-      </c>
-      <c r="K6" s="7">
-        <v>115</v>
-      </c>
-      <c r="L6" s="7">
-        <v>115</v>
-      </c>
-      <c r="M6" s="7">
-        <v>115</v>
-      </c>
-      <c r="N6" s="7">
-        <v>115</v>
-      </c>
-      <c r="O6" s="7">
-        <v>115</v>
-      </c>
-      <c r="P6" s="7">
-        <v>115</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>115</v>
-      </c>
-      <c r="R6" s="7">
-        <v>115</v>
-      </c>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3">
-        <v>76.099999999999994</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3">
-        <v>76.099999999999994</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3">
-        <v>90.1</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4">
-        <v>230.1</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3">
-        <v>152.1</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
-        <v>152.1</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3">
-        <v>152.1</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4">
-        <v>219.7</v>
-      </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>135</v>
-      </c>
-      <c r="D11">
-        <f>C11*1.2</f>
-        <v>162</v>
-      </c>
-      <c r="E11">
-        <v>180</v>
-      </c>
-      <c r="F11">
-        <f>E11*1.2</f>
-        <v>216</v>
-      </c>
-      <c r="G11">
-        <v>300</v>
-      </c>
-      <c r="H11">
-        <f>G11*1.2</f>
-        <v>360</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3">
         <v>18</v>
       </c>
       <c r="D12" s="3">
@@ -2865,8 +2984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639D0246-B22B-4F2A-9652-7A59722DF802}">
   <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3093,7 +3212,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4">
-        <v>779.3</v>
+        <v>798</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -3136,7 +3255,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4">
-        <v>1025.5</v>
+        <v>1235</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="2"/>
@@ -3474,11 +3593,1281 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88FA16E-2B64-4FB1-9A1C-0C3A0FCFEA76}">
+  <dimension ref="A1:S47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="E2" s="11">
+        <v>2</v>
+      </c>
+      <c r="F2" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="G2" s="11">
+        <v>3</v>
+      </c>
+      <c r="H2" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="I2" s="11">
+        <v>4</v>
+      </c>
+      <c r="J2" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="K2" s="11">
+        <v>5</v>
+      </c>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6">
+        <v>17.021999999999998</v>
+      </c>
+      <c r="D3" s="6">
+        <v>21.908850000000001</v>
+      </c>
+      <c r="E3" s="6">
+        <v>26.7957</v>
+      </c>
+      <c r="F3" s="6">
+        <v>31.682549999999999</v>
+      </c>
+      <c r="G3" s="6">
+        <v>36.569400000000002</v>
+      </c>
+      <c r="H3" s="6">
+        <v>41.456249999999997</v>
+      </c>
+      <c r="I3" s="6">
+        <v>46.3431</v>
+      </c>
+      <c r="J3" s="6">
+        <v>51.229950000000002</v>
+      </c>
+      <c r="K3" s="6">
+        <v>56.116799999999998</v>
+      </c>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11">
+        <v>2</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11">
+        <v>3</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11">
+        <v>4</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11">
+        <v>5</v>
+      </c>
+      <c r="J5" s="11">
+        <f>I5+0.5</f>
+        <v>5.5</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" ref="K5:R5" si="0">J5+0.5</f>
+        <v>6</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="M5" s="11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="O5" s="11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P5" s="11">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="Q5" s="11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R5" s="11">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="S5" s="11"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="11">
+        <v>17</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="14">
+        <v>51.747679964482344</v>
+      </c>
+      <c r="I6" s="14">
+        <v>55.617939999999997</v>
+      </c>
+      <c r="J6" s="4">
+        <v>62.358969999999999</v>
+      </c>
+      <c r="K6" s="4">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="L6" s="4">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="M6" s="4">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="N6" s="4">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="O6" s="4">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="P6" s="4">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="R6" s="13">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="S6" s="12"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="11">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
+        <v>35</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>52</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4">
+        <v>90</v>
+      </c>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="11">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3">
+        <v>70</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>70</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4">
+        <v>70</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4">
+        <v>115</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11">
+        <v>135</v>
+      </c>
+      <c r="D11" s="11">
+        <f>C11*1.2</f>
+        <v>162</v>
+      </c>
+      <c r="E11" s="11">
+        <v>180</v>
+      </c>
+      <c r="F11" s="11">
+        <f>E11*1.2</f>
+        <v>216</v>
+      </c>
+      <c r="G11" s="11">
+        <v>300</v>
+      </c>
+      <c r="H11" s="11">
+        <f>G11*1.2</f>
+        <v>360</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="11">
+        <v>17</v>
+      </c>
+      <c r="C12" s="7">
+        <v>29</v>
+      </c>
+      <c r="D12" s="7">
+        <v>32.642800000000001</v>
+      </c>
+      <c r="E12" s="7">
+        <v>36</v>
+      </c>
+      <c r="F12" s="7">
+        <v>41</v>
+      </c>
+      <c r="G12" s="7">
+        <v>52</v>
+      </c>
+      <c r="H12" s="7">
+        <v>61</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11">
+        <v>135</v>
+      </c>
+      <c r="D14" s="11">
+        <f>C14*1.2</f>
+        <v>162</v>
+      </c>
+      <c r="E14" s="11">
+        <v>180</v>
+      </c>
+      <c r="F14" s="11">
+        <f>E14*1.2</f>
+        <v>216</v>
+      </c>
+      <c r="G14" s="11">
+        <v>300</v>
+      </c>
+      <c r="H14" s="11">
+        <f>G14*1.2</f>
+        <v>360</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="11">
+        <v>17</v>
+      </c>
+      <c r="C15" s="7">
+        <v>63.6066</v>
+      </c>
+      <c r="D15" s="7">
+        <v>77.066100000000006</v>
+      </c>
+      <c r="E15" s="7">
+        <v>86.039100000000005</v>
+      </c>
+      <c r="F15" s="7">
+        <v>103.9851</v>
+      </c>
+      <c r="G15" s="7">
+        <v>145.85910000000001</v>
+      </c>
+      <c r="H15" s="7">
+        <v>175.76910000000001</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11">
+        <v>5</v>
+      </c>
+      <c r="D17" s="11">
+        <v>6</v>
+      </c>
+      <c r="E17" s="11">
+        <f>D17+1</f>
+        <v>7</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" ref="F17:N17" si="1">E17+1</f>
+        <v>8</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J17" s="11">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="L17" s="11">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="11">
+        <v>17</v>
+      </c>
+      <c r="C18" s="7">
+        <v>248.61250000000001</v>
+      </c>
+      <c r="D18" s="7">
+        <v>253.637</v>
+      </c>
+      <c r="E18" s="7">
+        <v>258.66149999999999</v>
+      </c>
+      <c r="F18" s="7">
+        <v>263.68600000000004</v>
+      </c>
+      <c r="G18" s="7">
+        <v>268.71050000000002</v>
+      </c>
+      <c r="H18" s="7">
+        <v>273.73500000000001</v>
+      </c>
+      <c r="I18" s="7">
+        <v>278.7595</v>
+      </c>
+      <c r="J18" s="7">
+        <v>283.78399999999999</v>
+      </c>
+      <c r="K18" s="7">
+        <v>288.80849999999998</v>
+      </c>
+      <c r="L18" s="7">
+        <v>293.83299999999997</v>
+      </c>
+      <c r="M18" s="7">
+        <v>298.85750000000002</v>
+      </c>
+      <c r="N18" s="7">
+        <v>303.88200000000001</v>
+      </c>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11">
+        <v>1</v>
+      </c>
+      <c r="D20" s="11">
+        <f>C20+1</f>
+        <v>2</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" ref="E20:G20" si="2">D20+1</f>
+        <v>3</v>
+      </c>
+      <c r="F20" s="11">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G20" s="11">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="11">
+        <v>16</v>
+      </c>
+      <c r="C21" s="5">
+        <v>18.2</v>
+      </c>
+      <c r="D21" s="5">
+        <v>18.2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>20.2</v>
+      </c>
+      <c r="F21" s="5">
+        <v>21.7</v>
+      </c>
+      <c r="G21" s="5">
+        <v>27.2</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11">
+        <v>300</v>
+      </c>
+      <c r="D23" s="11">
+        <v>800</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="11">
+        <v>22</v>
+      </c>
+      <c r="C24" s="5">
+        <v>72.5</v>
+      </c>
+      <c r="D24" s="5">
+        <v>145</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5D90EF-9577-46F9-8082-A1B922B07FFF}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4102,6 +5491,80 @@
         <v>1174</v>
       </c>
     </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27">
+        <v>1356.3</v>
+      </c>
+      <c r="D27">
+        <v>5514</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27">
+        <f>C27*D30</f>
+        <v>22.785839999999997</v>
+      </c>
+      <c r="I27">
+        <f>D27*D30</f>
+        <v>92.635199999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28">
+        <v>630</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28">
+        <f>D28*D31</f>
+        <v>85.050000000000011</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30">
+        <v>1.6799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31">
+        <v>0.13500000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>